<commit_message>
Organized simper pre comparison results
</commit_message>
<xml_diff>
--- a/Simper/Pre/stevia.pre_krusk_simper.xlsx
+++ b/Simper/Pre/stevia.pre_krusk_simper.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Li\Documents\Edna_GitHub\Stevia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Li\Documents\Edna_GitHub\Stevia\Simper\Pre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5CAD4344-3110-49BD-9B0B-8D8B902292C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB88E1-520A-4DF1-A2AD-AFB2C43FD717}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stevia.pre_krusk_simper" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Comparison</t>
   </si>
@@ -88,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -930,14 +938,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="87.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>